<commit_message>
Sua lai db va them note
</commit_message>
<xml_diff>
--- a/BTL/Note/MauDB.xlsx
+++ b/BTL/Note/MauDB.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://utcedu-my.sharepoint.com/personal/dat181200376_st_utc_edu_vn/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MS_visual_studio\project\BTL-LTTQ\BTL\Note\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F8F012D3-46D9-450C-8EBF-98BB1BD03D78}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F41F340-03E3-4F0D-BF05-EB8C3E9FF34D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6564" yWindow="528" windowWidth="16248" windowHeight="10656" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6504" yWindow="1308" windowWidth="16248" windowHeight="10656" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Trang_tính1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191028" calcCompleted="0"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="118">
   <si>
     <t>Đề tài: Quản lý cửa hàng bán đồ ăn nhanh</t>
   </si>
@@ -177,9 +178,6 @@
     <t>Tên nguyên liệu ( TênNL )</t>
   </si>
   <si>
-    <t xml:space="preserve">Tên nhân viên </t>
-  </si>
-  <si>
     <t>Mã nhà cung cấp (idCC)</t>
   </si>
   <si>
@@ -253,13 +251,151 @@
   </si>
   <si>
     <t>//Số lượng sẽ bằng còn + nhập</t>
+  </si>
+  <si>
+    <t>idNV</t>
+  </si>
+  <si>
+    <t>hotenNV</t>
+  </si>
+  <si>
+    <t>ngaySinh</t>
+  </si>
+  <si>
+    <t>imgNV</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>soDT</t>
+  </si>
+  <si>
+    <t>chucVu</t>
+  </si>
+  <si>
+    <t>NV01</t>
+  </si>
+  <si>
+    <t>NV01.jpg</t>
+  </si>
+  <si>
+    <t>Thu Ngân</t>
+  </si>
+  <si>
+    <t>NV02</t>
+  </si>
+  <si>
+    <t>NV03</t>
+  </si>
+  <si>
+    <t>NV04</t>
+  </si>
+  <si>
+    <t>NV05</t>
+  </si>
+  <si>
+    <t>Giới tính</t>
+  </si>
+  <si>
+    <t>NV02.jpg</t>
+  </si>
+  <si>
+    <t>NV03.jpg</t>
+  </si>
+  <si>
+    <t>NV04.jpg</t>
+  </si>
+  <si>
+    <t>NV05.jpg</t>
+  </si>
+  <si>
+    <t>Đặng Tuấn Đạt</t>
+  </si>
+  <si>
+    <t>Admin</t>
+  </si>
+  <si>
+    <t>Quản lý</t>
+  </si>
+  <si>
+    <t>Nam</t>
+  </si>
+  <si>
+    <t>Trần Văn Minh</t>
+  </si>
+  <si>
+    <t>tranvm@gmail.com</t>
+  </si>
+  <si>
+    <t>Vũ Hữu Tuấn</t>
+  </si>
+  <si>
+    <t>vuht@gmail.com</t>
+  </si>
+  <si>
+    <t>Trang Phi Hung</t>
+  </si>
+  <si>
+    <t>trang@gmail.com</t>
+  </si>
+  <si>
+    <t>Phục vụ</t>
+  </si>
+  <si>
+    <t>Pham Hoai Bong</t>
+  </si>
+  <si>
+    <t>phamHB@gmail.com</t>
+  </si>
+  <si>
+    <t>dtd@gmail.com</t>
+  </si>
+  <si>
+    <t>KH01</t>
+  </si>
+  <si>
+    <t>Đỗ Thanh Hàn</t>
+  </si>
+  <si>
+    <t>Hà Nội</t>
+  </si>
+  <si>
+    <t>KH02</t>
+  </si>
+  <si>
+    <t>Đăng Huyền Sinh</t>
+  </si>
+  <si>
+    <t>Hà Tĩnh</t>
+  </si>
+  <si>
+    <t>KH03</t>
+  </si>
+  <si>
+    <t>Nguyễn Quang Huy</t>
+  </si>
+  <si>
+    <t>Nghệ An</t>
+  </si>
+  <si>
+    <t>idKH</t>
+  </si>
+  <si>
+    <t>hoTenKH</t>
+  </si>
+  <si>
+    <t>diaChi</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
+  </numFmts>
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -306,8 +442,21 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="14"/>
+      <color theme="4"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -323,6 +472,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -367,7 +528,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -382,12 +543,30 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Bình thường" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -701,34 +880,34 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:J38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="18"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="18" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="9" style="1"/>
-    <col min="2" max="2" width="32.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="32.33203125" style="1" customWidth="1"/>
     <col min="3" max="4" width="9" style="1"/>
-    <col min="5" max="5" width="36.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="36.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9" style="1"/>
-    <col min="7" max="7" width="36.28515625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="36.33203125" style="1" customWidth="1"/>
     <col min="8" max="9" width="9" style="1"/>
-    <col min="10" max="10" width="30.7109375" style="1" customWidth="1"/>
+    <col min="10" max="10" width="30.6640625" style="1" customWidth="1"/>
     <col min="11" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10">
-      <c r="B2" s="14" t="s">
+    <row r="2" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B2" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="14"/>
-    </row>
-    <row r="4" spans="2:10">
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B4" s="2" t="s">
         <v>1</v>
       </c>
@@ -742,7 +921,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="2:10">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B5" s="3" t="s">
         <v>5</v>
       </c>
@@ -756,7 +935,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="2:10">
+    <row r="6" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B6" s="4" t="s">
         <v>9</v>
       </c>
@@ -766,11 +945,11 @@
       <c r="G6" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="J6" s="4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="2:10">
+      <c r="J6" s="24" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B7" s="4" t="s">
         <v>13</v>
       </c>
@@ -781,10 +960,10 @@
         <v>15</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="2:10">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B8" s="4" t="s">
         <v>17</v>
       </c>
@@ -795,10 +974,10 @@
         <v>19</v>
       </c>
       <c r="J8" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="2:10">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B9" s="4" t="s">
         <v>21</v>
       </c>
@@ -808,35 +987,35 @@
       <c r="G9" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="J9" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="10" spans="2:10">
+      <c r="J9" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B10" s="4" t="s">
         <v>18</v>
       </c>
       <c r="E10" s="4" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="11" spans="2:10">
+      <c r="J10" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B11" s="4" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="2:10">
+    <row r="12" spans="2:10" x14ac:dyDescent="0.35">
       <c r="E12" s="2" t="s">
         <v>26</v>
       </c>
       <c r="G12" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="J12" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="13" spans="2:10">
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B13" s="2" t="s">
         <v>29</v>
       </c>
@@ -846,11 +1025,11 @@
       <c r="G13" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="J13" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="14" spans="2:10">
+      <c r="J13" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B14" s="3" t="s">
         <v>11</v>
       </c>
@@ -858,11 +1037,11 @@
       <c r="G14" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="J14" s="13" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="15" spans="2:10">
+      <c r="J14" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B15" s="4" t="s">
         <v>32</v>
       </c>
@@ -872,8 +1051,11 @@
       <c r="G15" s="4" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="16" spans="2:10">
+      <c r="J15" s="13" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B16" s="4" t="s">
         <v>34</v>
       </c>
@@ -884,7 +1066,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="17" spans="2:10">
+    <row r="17" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B17" s="4" t="s">
         <v>36</v>
       </c>
@@ -895,17 +1077,17 @@
         <v>38</v>
       </c>
     </row>
-    <row r="18" spans="2:10">
+    <row r="18" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B18" s="4" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="19" spans="2:10">
+    <row r="19" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B19" s="6" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="20" spans="2:10">
+    <row r="20" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B20" s="4" t="s">
         <v>41</v>
       </c>
@@ -915,22 +1097,19 @@
       <c r="G20" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="J20" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="21" spans="2:10">
+    </row>
+    <row r="21" spans="2:10" x14ac:dyDescent="0.35">
       <c r="E21" s="5" t="s">
         <v>11</v>
       </c>
       <c r="G21" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="J21" s="12" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="22" spans="2:10">
+      <c r="J21" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="22" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B22" s="2" t="s">
         <v>46</v>
       </c>
@@ -940,144 +1119,145 @@
       <c r="G22" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="J22" s="11" t="s">
+      <c r="J22" s="12" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="23" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B23" s="3" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="23" spans="2:10">
-      <c r="B23" s="3" t="s">
+      <c r="G23" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="G23" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="J23" s="4" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="24" spans="2:10">
+      <c r="J23" s="11"/>
+    </row>
+    <row r="24" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B24" s="4" t="s">
         <v>21</v>
       </c>
       <c r="G24" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="J24" s="4" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="25" spans="2:10">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="25" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B25" s="4" t="s">
         <v>18</v>
       </c>
       <c r="E25" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="G25" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="G25" s="1" t="s">
+      <c r="J25" s="4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="26" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B26" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="J26" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="J25" s="4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="26" spans="2:10">
-      <c r="B26" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="E26" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="J26" s="10"/>
-    </row>
-    <row r="27" spans="2:10">
+    </row>
+    <row r="27" spans="2:10" x14ac:dyDescent="0.35">
       <c r="E27" s="3" t="s">
         <v>5</v>
       </c>
       <c r="G27" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="J27" s="10"/>
+    </row>
+    <row r="28" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B28" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="J27" s="10"/>
-    </row>
-    <row r="28" spans="2:10">
-      <c r="B28" s="2" t="s">
+      <c r="E28" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="G28" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="E28" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="G28" s="7" t="s">
+      <c r="J28" s="10"/>
+    </row>
+    <row r="29" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B29" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="E29" s="4" t="s">
         <v>61</v>
-      </c>
-    </row>
-    <row r="29" spans="2:10">
-      <c r="B29" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="E29" s="4" t="s">
-        <v>62</v>
       </c>
       <c r="G29" s="5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="30" spans="2:10">
+    <row r="30" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B30" s="3" t="s">
         <v>45</v>
       </c>
       <c r="E30" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="G30" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="G30" s="9" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="31" spans="2:10">
+    </row>
+    <row r="31" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B31" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E31" s="4" t="s">
         <v>39</v>
       </c>
       <c r="G31" s="4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="32" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B32" s="4" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="32" spans="2:10">
-      <c r="B32" s="4" t="s">
+      <c r="G32" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="G32" s="4" t="s">
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B33" s="4" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="33" spans="2:2">
-      <c r="B33" s="4" t="s">
+    <row r="34" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B34" s="1" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="34" spans="2:2">
-      <c r="B34" s="1" t="s">
+    <row r="35" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B35" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="35" spans="2:2">
-      <c r="B35" s="1" t="s">
+    <row r="36" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B36" s="1" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="36" spans="2:2">
-      <c r="B36" s="1" t="s">
+    <row r="37" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B37" s="1" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="37" spans="2:2">
-      <c r="B37" s="1" t="s">
+    <row r="38" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B38" s="1" t="s">
         <v>72</v>
-      </c>
-    </row>
-    <row r="38" spans="2:2">
-      <c r="B38" s="1" t="s">
-        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -1087,4 +1267,287 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80BDBB69-007B-414F-B693-453E4C6FB80D}">
+  <dimension ref="A2:I15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="6.109375" customWidth="1"/>
+    <col min="3" max="3" width="17.33203125" customWidth="1"/>
+    <col min="4" max="4" width="13.21875" customWidth="1"/>
+    <col min="5" max="5" width="12" customWidth="1"/>
+    <col min="6" max="6" width="19.5546875" customWidth="1"/>
+    <col min="7" max="7" width="16.77734375" customWidth="1"/>
+    <col min="8" max="8" width="10.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" s="23">
+        <v>1</v>
+      </c>
+      <c r="B2" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="C2" s="19" t="s">
+        <v>74</v>
+      </c>
+      <c r="D2" s="19" t="s">
+        <v>75</v>
+      </c>
+      <c r="E2" s="19" t="s">
+        <v>76</v>
+      </c>
+      <c r="F2" s="19" t="s">
+        <v>77</v>
+      </c>
+      <c r="G2" s="19" t="s">
+        <v>78</v>
+      </c>
+      <c r="H2" s="19" t="s">
+        <v>79</v>
+      </c>
+      <c r="I2" s="19" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B3" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="C3" s="20" t="s">
+        <v>96</v>
+      </c>
+      <c r="D3" s="21">
+        <v>27503</v>
+      </c>
+      <c r="E3" s="20" t="s">
+        <v>81</v>
+      </c>
+      <c r="F3" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="G3" s="20">
+        <v>123456789</v>
+      </c>
+      <c r="H3" s="20" t="s">
+        <v>82</v>
+      </c>
+      <c r="I3" s="22" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B4" s="20" t="s">
+        <v>83</v>
+      </c>
+      <c r="C4" s="20" t="s">
+        <v>98</v>
+      </c>
+      <c r="D4" s="21">
+        <v>27681</v>
+      </c>
+      <c r="E4" s="20" t="s">
+        <v>88</v>
+      </c>
+      <c r="F4" s="20" t="s">
+        <v>99</v>
+      </c>
+      <c r="G4" s="20">
+        <v>9075403151</v>
+      </c>
+      <c r="H4" s="20" t="s">
+        <v>94</v>
+      </c>
+      <c r="I4" s="22" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B5" s="20" t="s">
+        <v>84</v>
+      </c>
+      <c r="C5" s="20" t="s">
+        <v>100</v>
+      </c>
+      <c r="D5" s="21">
+        <v>27702</v>
+      </c>
+      <c r="E5" s="20" t="s">
+        <v>89</v>
+      </c>
+      <c r="F5" s="20" t="s">
+        <v>101</v>
+      </c>
+      <c r="G5" s="20">
+        <v>3189605845</v>
+      </c>
+      <c r="H5" s="20" t="s">
+        <v>102</v>
+      </c>
+      <c r="I5" s="22" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="20" t="s">
+        <v>85</v>
+      </c>
+      <c r="C6" s="20" t="s">
+        <v>103</v>
+      </c>
+      <c r="D6" s="21">
+        <v>26950</v>
+      </c>
+      <c r="E6" s="20" t="s">
+        <v>90</v>
+      </c>
+      <c r="F6" s="20" t="s">
+        <v>104</v>
+      </c>
+      <c r="G6" s="20">
+        <v>1850482092</v>
+      </c>
+      <c r="H6" s="20" t="s">
+        <v>102</v>
+      </c>
+      <c r="I6" s="22" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B7" s="20" t="s">
+        <v>86</v>
+      </c>
+      <c r="C7" s="20" t="s">
+        <v>92</v>
+      </c>
+      <c r="D7" s="21">
+        <v>27398</v>
+      </c>
+      <c r="E7" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="F7" s="20" t="s">
+        <v>105</v>
+      </c>
+      <c r="G7" s="20">
+        <v>7618614247</v>
+      </c>
+      <c r="H7" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="I7" s="22" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B8" s="14"/>
+      <c r="C8" s="14"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="14"/>
+      <c r="G8" s="14"/>
+      <c r="H8" s="14"/>
+      <c r="I8" s="14"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B9" s="16"/>
+      <c r="C9" s="16"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="16"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="16"/>
+      <c r="H9" s="16"/>
+      <c r="I9" s="16"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A11" s="23">
+        <v>2</v>
+      </c>
+      <c r="B11" s="19" t="s">
+        <v>115</v>
+      </c>
+      <c r="C11" s="19" t="s">
+        <v>116</v>
+      </c>
+      <c r="D11" s="19" t="s">
+        <v>117</v>
+      </c>
+      <c r="E11" s="19" t="s">
+        <v>78</v>
+      </c>
+      <c r="F11" s="19" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B12" s="20" t="s">
+        <v>106</v>
+      </c>
+      <c r="C12" s="20" t="s">
+        <v>107</v>
+      </c>
+      <c r="D12" s="20" t="s">
+        <v>108</v>
+      </c>
+      <c r="E12" s="20">
+        <v>5576373380</v>
+      </c>
+      <c r="F12" s="21">
+        <v>27499</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B13" s="20" t="s">
+        <v>109</v>
+      </c>
+      <c r="C13" s="20" t="s">
+        <v>110</v>
+      </c>
+      <c r="D13" s="20" t="s">
+        <v>111</v>
+      </c>
+      <c r="E13" s="20">
+        <v>9577987459</v>
+      </c>
+      <c r="F13" s="21">
+        <v>27269</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B14" s="20" t="s">
+        <v>112</v>
+      </c>
+      <c r="C14" s="20" t="s">
+        <v>113</v>
+      </c>
+      <c r="D14" s="20" t="s">
+        <v>114</v>
+      </c>
+      <c r="E14" s="20">
+        <v>7958610097</v>
+      </c>
+      <c r="F14" s="21">
+        <v>27626</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B15" s="19"/>
+      <c r="C15" s="19"/>
+      <c r="D15" s="19"/>
+      <c r="E15" s="19"/>
+      <c r="F15" s="19"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="7" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Chinh sua ngay 11/11
</commit_message>
<xml_diff>
--- a/BTL/Note/MauDB.xlsx
+++ b/BTL/Note/MauDB.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MS_visual_studio\project\BTL-LTTQ\BTL\Note\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MS_visual_studio\project\BTL-LTTQ-QUANLIDOAN\BTL\Note\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84BAF303-119A-4514-9634-37A295B72ECA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31804779-D82D-4236-BFA9-2D56D4B19ABA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6504" yWindow="1308" windowWidth="16248" windowHeight="10656" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="108">
   <si>
     <t>Đề tài: Quản lý cửa hàng bán đồ ăn nhanh</t>
   </si>
@@ -187,31 +187,16 @@
     <t>Mã chi tiết (idDetail)</t>
   </si>
   <si>
-    <t xml:space="preserve">Combo sản phẩm </t>
-  </si>
-  <si>
     <t>Chi tiết Nguyên liệu</t>
   </si>
   <si>
-    <t xml:space="preserve">Mã combo (idCombo) </t>
-  </si>
-  <si>
     <t>Ngày tạo hóa đơn nhập (DateHD)</t>
   </si>
   <si>
     <t>Số lượng (Count)</t>
   </si>
   <si>
-    <t>Hình ảnh ( imageCombo)</t>
-  </si>
-  <si>
-    <t>Tổng tiền</t>
-  </si>
-  <si>
     <t>Số lượng  (Count)</t>
-  </si>
-  <si>
-    <t>Chi tiết (Description)</t>
   </si>
   <si>
     <t xml:space="preserve">Tình trạng (Status) </t>
@@ -546,11 +531,11 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -867,8 +852,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:K39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J32" sqref="J32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="18" x14ac:dyDescent="0.35"/>
@@ -886,30 +871,30 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
-      <c r="G2" s="24"/>
-      <c r="H2" s="24"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
+      <c r="G2" s="26"/>
+      <c r="H2" s="26"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A4" s="25"/>
+      <c r="A4" s="24"/>
       <c r="B4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="26"/>
+      <c r="D4" s="25"/>
       <c r="E4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="26"/>
+      <c r="G4" s="25"/>
       <c r="H4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="J4" s="26"/>
+      <c r="J4" s="25"/>
       <c r="K4" s="2" t="s">
         <v>4</v>
       </c>
@@ -999,17 +984,17 @@
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="D12" s="26"/>
+      <c r="D12" s="25"/>
       <c r="E12" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="G12" s="26"/>
+      <c r="G12" s="25"/>
       <c r="H12" s="2" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A13" s="26"/>
+      <c r="A13" s="25"/>
       <c r="B13" s="2" t="s">
         <v>27</v>
       </c>
@@ -1069,7 +1054,7 @@
         <v>36</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.35">
@@ -1081,11 +1066,11 @@
       <c r="B20" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="D20" s="26"/>
+      <c r="D20" s="25"/>
       <c r="E20" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="G20" s="26"/>
+      <c r="G20" s="25"/>
       <c r="H20" s="2" t="s">
         <v>40</v>
       </c>
@@ -1097,11 +1082,11 @@
       <c r="H21" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="J21" s="26"/>
+      <c r="J21" s="25"/>
       <c r="K21" s="2"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A22" s="26"/>
+      <c r="A22" s="25"/>
       <c r="B22" s="2" t="s">
         <v>42</v>
       </c>
@@ -1135,7 +1120,7 @@
       <c r="B25" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D25" s="26"/>
+      <c r="D25" s="25"/>
       <c r="E25" s="2" t="s">
         <v>47</v>
       </c>
@@ -1157,23 +1142,19 @@
       <c r="E27" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="G27" s="26"/>
-      <c r="H27" s="2" t="s">
+      <c r="G27" s="25"/>
+      <c r="H27" s="2"/>
+      <c r="K27" s="10"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A28" s="25"/>
+      <c r="B28" s="2" t="s">
         <v>51</v>
-      </c>
-      <c r="K27" s="10"/>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A28" s="26"/>
-      <c r="B28" s="2" t="s">
-        <v>52</v>
       </c>
       <c r="E28" s="23" t="s">
         <v>44</v>
       </c>
-      <c r="H28" s="7" t="s">
-        <v>53</v>
-      </c>
+      <c r="H28" s="7"/>
       <c r="K28" s="10"/>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.35">
@@ -1181,7 +1162,7 @@
         <v>50</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="H29" s="5"/>
     </row>
@@ -1190,11 +1171,9 @@
         <v>41</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="H30" s="9" t="s">
-        <v>56</v>
-      </c>
+        <v>53</v>
+      </c>
+      <c r="H30" s="9"/>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B31" s="4" t="s">
@@ -1203,51 +1182,47 @@
       <c r="E31" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="H31" s="4" t="s">
-        <v>57</v>
-      </c>
+      <c r="H31" s="4"/>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B32" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="H32" s="4" t="s">
-        <v>59</v>
-      </c>
+        <v>54</v>
+      </c>
+      <c r="H32" s="4"/>
     </row>
     <row r="33" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B33" s="4" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
     </row>
     <row r="34" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B34" s="1" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="35" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B35" s="1" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
     </row>
     <row r="36" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B36" s="1" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
     </row>
     <row r="37" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B37" s="1" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="38" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B38" s="1" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
     </row>
     <row r="39" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B39" s="1" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
     </row>
   </sheetData>
@@ -1283,158 +1258,158 @@
         <v>1</v>
       </c>
       <c r="B2" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="C2" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="D2" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="E2" s="18" t="s">
+        <v>64</v>
+      </c>
+      <c r="F2" s="18" t="s">
+        <v>65</v>
+      </c>
+      <c r="G2" s="18" t="s">
         <v>66</v>
       </c>
-      <c r="C2" s="18" t="s">
+      <c r="H2" s="18" t="s">
         <v>67</v>
       </c>
-      <c r="D2" s="18" t="s">
-        <v>68</v>
-      </c>
-      <c r="E2" s="18" t="s">
-        <v>69</v>
-      </c>
-      <c r="F2" s="18" t="s">
-        <v>70</v>
-      </c>
-      <c r="G2" s="18" t="s">
-        <v>71</v>
-      </c>
-      <c r="H2" s="18" t="s">
-        <v>72</v>
-      </c>
       <c r="I2" s="18" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B3" s="19" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="C3" s="19" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="D3" s="20">
         <v>27503</v>
       </c>
       <c r="E3" s="19" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="F3" s="19" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="G3" s="19">
         <v>123456789</v>
       </c>
       <c r="H3" s="19" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="I3" s="21" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B4" s="19" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="C4" s="19" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="D4" s="20">
         <v>27681</v>
       </c>
       <c r="E4" s="19" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="F4" s="19" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="G4" s="19">
         <v>9075403151</v>
       </c>
       <c r="H4" s="19" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="I4" s="21" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B5" s="19" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="C5" s="19" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="D5" s="20">
         <v>27702</v>
       </c>
       <c r="E5" s="19" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="F5" s="19" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="G5" s="19">
         <v>3189605845</v>
       </c>
       <c r="H5" s="19" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="I5" s="21" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="19" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="C6" s="19" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="D6" s="20">
         <v>26950</v>
       </c>
       <c r="E6" s="19" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="F6" s="19" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="G6" s="19">
         <v>1850482092</v>
       </c>
       <c r="H6" s="19" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="I6" s="21" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B7" s="19" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="C7" s="19" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="D7" s="20">
         <v>27398</v>
       </c>
       <c r="E7" s="19" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="F7" s="19" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="G7" s="19">
         <v>7618614247</v>
       </c>
       <c r="H7" s="19" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="I7" s="21" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
@@ -1462,30 +1437,30 @@
         <v>2</v>
       </c>
       <c r="B11" s="18" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="C11" s="18" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="D11" s="18" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="E11" s="18" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="F11" s="18" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B12" s="19" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="C12" s="19" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="D12" s="19" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="E12" s="19">
         <v>5576373380</v>
@@ -1496,13 +1471,13 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B13" s="19" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="C13" s="19" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="D13" s="19" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="E13" s="19">
         <v>9577987459</v>
@@ -1513,13 +1488,13 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B14" s="19" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="C14" s="19" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="D14" s="19" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="E14" s="19">
         <v>7958610097</v>

</xml_diff>